<commit_message>
Update 6 - Runge-Kutta 4ta ordem.xlsx
</commit_message>
<xml_diff>
--- a/Prova 2/6 - Runge-Kutta 4ta ordem.xlsx
+++ b/Prova 2/6 - Runge-Kutta 4ta ordem.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCAS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCAS\Documents\GitHub\Trabalho_Metodos_numericos\Prova 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Qual valor de u(1)?</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>k4</t>
+  </si>
+  <si>
+    <t>testesteste</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:DD1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -802,7 +805,9 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="M15" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1760,7 +1765,7 @@
         <v>0.98000000000000065</v>
       </c>
       <c r="CX27" s="2">
-        <f t="shared" ref="CX27:DC27" si="17">CW27+$C$26</f>
+        <f t="shared" ref="CX27:CY27" si="17">CW27+$C$26</f>
         <v>0.99000000000000066</v>
       </c>
       <c r="CY27" s="2">
@@ -2174,7 +2179,7 @@
         <v>6.9140707579265612</v>
       </c>
       <c r="CX28" s="2">
-        <f t="shared" ref="CX28:DC28" si="29">CW28+1/6*(CW29+2*CW30+2*CW31+CW32)*$C$26</f>
+        <f t="shared" ref="CX28:CY28" si="29">CW28+1/6*(CW29+2*CW30+2*CW31+CW32)*$C$26</f>
         <v>6.909909471013183</v>
       </c>
       <c r="CY28" s="2">
@@ -2193,7 +2198,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" ref="C29:M29" si="30">-0.5*C28+2+C27</f>
+        <f t="shared" ref="C29:D29" si="30">-0.5*C28+2+C27</f>
         <v>-2</v>
       </c>
       <c r="D29" s="2">
@@ -2453,7 +2458,7 @@
         <v>-0.92498121238037823</v>
       </c>
       <c r="BP29" s="2">
-        <f t="shared" ref="BP29:DD29" si="34">-0.5*BP28+2+BP27</f>
+        <f t="shared" ref="BP29:CY29" si="34">-0.5*BP28+2+BP27</f>
         <v>-0.91071591143055031</v>
       </c>
       <c r="BQ29" s="2">
@@ -2611,7 +2616,7 @@
         <v>-1.9900000000000002</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" ref="C30:M30" si="35">-0.5*(D28+1/2*D29*$C$16)+2+(D27+1/2*$C$16)</f>
+        <f t="shared" ref="D30" si="35">-0.5*(D28+1/2*D29*$C$16)+2+(D27+1/2*$C$16)</f>
         <v>-1.8805486688515627</v>
       </c>
       <c r="E30" s="2">
@@ -2867,7 +2872,7 @@
         <v>-0.85185668207086884</v>
       </c>
       <c r="BP30" s="2">
-        <f t="shared" ref="BP30:DD30" si="39">-0.5*(BP28+1/2*BP29*$C$16)+2+(BP27+1/2*$C$16)</f>
+        <f t="shared" ref="BP30:CY30" si="39">-0.5*(BP28+1/2*BP29*$C$16)+2+(BP27+1/2*$C$16)</f>
         <v>-0.83794801364478633</v>
       </c>
       <c r="BQ30" s="2">
@@ -3025,7 +3030,7 @@
         <v>-1.9900250000000002</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ref="C31:M31" si="40">-0.5*(D28+1/2*D30*$C$16)+2+(D27+1/2*$C$16)</f>
+        <f t="shared" ref="D31" si="40">-0.5*(D28+1/2*D30*$C$16)+2+(D27+1/2*$C$16)</f>
         <v>-1.8830362000495442</v>
       </c>
       <c r="E31" s="2">
@@ -3281,7 +3286,7 @@
         <v>-0.85368479532860642</v>
       </c>
       <c r="BP31" s="2">
-        <f t="shared" ref="BP31:DD31" si="44">-0.5*(BP28+1/2*BP30*$C$16)+2+(BP27+1/2*$C$16)</f>
+        <f t="shared" ref="BP31:CY31" si="44">-0.5*(BP28+1/2*BP30*$C$16)+2+(BP27+1/2*$C$16)</f>
         <v>-0.83976721108943075</v>
       </c>
       <c r="BQ31" s="2">
@@ -3439,7 +3444,7 @@
         <v>-1.980049875</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" ref="C32:M32" si="45">-0.5*(D28+D31*$C$16)+2+(D27+$C$16)</f>
+        <f t="shared" ref="D32" si="45">-0.5*(D28+D31*$C$16)+2+(D27+$C$16)</f>
         <v>-1.7858981067683561</v>
       </c>
       <c r="E32" s="2">
@@ -3695,7 +3700,7 @@
         <v>-0.78229697261394804</v>
       </c>
       <c r="BP32" s="2">
-        <f t="shared" ref="BP32:DD32" si="49">-0.5*(BP28+BP31*$C$16)+2+(BP27+$C$16)</f>
+        <f t="shared" ref="BP32:CY32" si="49">-0.5*(BP28+BP31*$C$16)+2+(BP27+$C$16)</f>
         <v>-0.7687275508760788</v>
       </c>
       <c r="BQ32" s="2">

</xml_diff>

<commit_message>
Coloquei os outros xlsx
</commit_message>
<xml_diff>
--- a/Prova 2/6 - Runge-Kutta 4ta ordem.xlsx
+++ b/Prova 2/6 - Runge-Kutta 4ta ordem.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t>Qual valor de u(1)?</t>
   </si>
@@ -104,13 +104,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -144,7 +147,7 @@
         <xdr:cNvPr id="2" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -178,7 +181,7 @@
         <xdr:cNvPr id="3" name="image3.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -216,7 +219,7 @@
         <xdr:cNvPr id="4" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -254,7 +257,7 @@
         <xdr:cNvPr id="5" name="image3.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -485,8 +488,8 @@
   </sheetPr>
   <dimension ref="A1:ANV1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3935,6 +3938,12 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:1062" x14ac:dyDescent="0.2">
+      <c r="E34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <v>6.9058660200803219</v>
+      </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -7935,7 +7944,7 @@
         <v>0.97900000000000076</v>
       </c>
       <c r="AKU37" s="2">
-        <f t="shared" ref="AKU37:ANF37" si="67">AKT37+$C$36</f>
+        <f t="shared" ref="AKU37:ALO37" si="67">AKT37+$C$36</f>
         <v>0.98000000000000076</v>
       </c>
       <c r="AKV37" s="2">
@@ -12003,7 +12012,7 @@
         <v>6.861462271780586</v>
       </c>
       <c r="AKU38" s="2">
-        <f t="shared" ref="AKU38:ANF38" si="85">AKT38+1/6*(AKT39+2*AKT40+2*AKT41+AKT42)*$C$36</f>
+        <f t="shared" ref="AKU38:ALO38" si="85">AKT38+1/6*(AKT39+2*AKT40+2*AKT41+AKT42)*$C$36</f>
         <v>6.8610111534753369</v>
       </c>
       <c r="AKV38" s="2">
@@ -12152,7 +12161,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="2">
-        <f t="shared" ref="C39:M39" si="86">-0.5*C38+2+C37</f>
+        <f t="shared" ref="C39" si="86">-0.5*C38+2+C37</f>
         <v>-2</v>
       </c>
       <c r="D39" s="2">
@@ -16072,7 +16081,7 @@
         <v>-0.45173113589029223</v>
       </c>
       <c r="AKU39" s="2">
-        <f t="shared" ref="AKU39:ANF39" si="104">-0.5*AKU38+2+AKU37</f>
+        <f t="shared" ref="AKU39:ALO39" si="104">-0.5*AKU38+2+AKU37</f>
         <v>-0.45050557673766767</v>
       </c>
       <c r="AKV39" s="2">

</xml_diff>